<commit_message>
subimos el último SPA
</commit_message>
<xml_diff>
--- a/data/output/Pedido_Semana_07_21022026_deco_exterior.xlsx
+++ b/data/output/Pedido_Semana_07_21022026_deco_exterior.xlsx
@@ -820,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="R4" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4" s="2" t="n">
         <v>0</v>
@@ -2262,7 +2262,7 @@
         <v>24</v>
       </c>
       <c r="R22" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S22" s="2" t="n">
         <v>0</v>
@@ -2343,16 +2343,16 @@
         <v>12</v>
       </c>
       <c r="R23" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S23" s="2" t="n">
         <v>1</v>
       </c>
       <c r="T23" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U23" s="8" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24">
@@ -2505,13 +2505,13 @@
         <v>0</v>
       </c>
       <c r="R25" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S25" s="2" t="n">
         <v>1</v>
       </c>
       <c r="T25" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U25" s="8" t="n">
         <v>0</v>
@@ -3558,13 +3558,13 @@
         <v>0</v>
       </c>
       <c r="R38" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S38" s="2" t="n">
         <v>6</v>
       </c>
       <c r="T38" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="U38" s="8" t="n">
         <v>0</v>
@@ -3639,13 +3639,13 @@
         <v>0</v>
       </c>
       <c r="R39" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S39" s="2" t="n">
         <v>9</v>
       </c>
       <c r="T39" s="3" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="U39" s="8" t="n">
         <v>0</v>
@@ -4206,13 +4206,13 @@
         <v>0</v>
       </c>
       <c r="R46" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S46" s="2" t="n">
         <v>3</v>
       </c>
       <c r="T46" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U46" s="8" t="n">
         <v>0</v>
@@ -4287,7 +4287,7 @@
         <v>3</v>
       </c>
       <c r="R47" s="2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S47" s="2" t="n">
         <v>0</v>
@@ -4692,13 +4692,13 @@
         <v>0</v>
       </c>
       <c r="R52" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S52" s="2" t="n">
         <v>8</v>
       </c>
       <c r="T52" s="3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U52" s="8" t="n">
         <v>0</v>
@@ -4854,7 +4854,7 @@
         <v>0</v>
       </c>
       <c r="R54" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S54" s="2" t="n">
         <v>0</v>
@@ -5583,13 +5583,13 @@
         <v>0</v>
       </c>
       <c r="R63" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S63" s="2" t="n">
         <v>3</v>
       </c>
       <c r="T63" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U63" s="8" t="n">
         <v>0</v>
@@ -6015,7 +6015,7 @@
         </is>
       </c>
       <c r="C71" s="5" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72">

</xml_diff>